<commit_message>
updated pytest and resized widget GUI
</commit_message>
<xml_diff>
--- a/lotr_form.xlsx
+++ b/lotr_form.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="168">
   <si>
     <t>Company</t>
   </si>
@@ -46,7 +46,7 @@
     <t>Baggin</t>
   </si>
   <si>
-    <t>12 bag end</t>
+    <t>4 bag end</t>
   </si>
   <si>
     <t>WestFarthing</t>
@@ -311,6 +311,210 @@
   </si>
   <si>
     <t>555-000-1111</t>
+  </si>
+  <si>
+    <t>Tom's Farm</t>
+  </si>
+  <si>
+    <t>Tom</t>
+  </si>
+  <si>
+    <t>Bombadil</t>
+  </si>
+  <si>
+    <t>500 Forest Road</t>
+  </si>
+  <si>
+    <t>Old Forest</t>
+  </si>
+  <si>
+    <t>Tom@tomsfarm.com</t>
+  </si>
+  <si>
+    <t>555-222-3333</t>
+  </si>
+  <si>
+    <t>Moria Mining</t>
+  </si>
+  <si>
+    <t>Balin</t>
+  </si>
+  <si>
+    <t>Son of Fundin</t>
+  </si>
+  <si>
+    <t>100 Deep Delve</t>
+  </si>
+  <si>
+    <t>Moria</t>
+  </si>
+  <si>
+    <t>Balin@moriemining.com</t>
+  </si>
+  <si>
+    <t>Ent Tree Care</t>
+  </si>
+  <si>
+    <t>Treebeard</t>
+  </si>
+  <si>
+    <t>Ent</t>
+  </si>
+  <si>
+    <t>1 Forest Path</t>
+  </si>
+  <si>
+    <t>Fangorn</t>
+  </si>
+  <si>
+    <t>Entwood</t>
+  </si>
+  <si>
+    <t>Treebeard@entcare.com</t>
+  </si>
+  <si>
+    <t>555-444-5555</t>
+  </si>
+  <si>
+    <t>Eagle Transport</t>
+  </si>
+  <si>
+    <t>Gwaihir</t>
+  </si>
+  <si>
+    <t>Windlord</t>
+  </si>
+  <si>
+    <t>1000 Sky Way</t>
+  </si>
+  <si>
+    <t>Eyrie</t>
+  </si>
+  <si>
+    <t>Misty Mountains</t>
+  </si>
+  <si>
+    <t>Gwaihir@eagletransport.com</t>
+  </si>
+  <si>
+    <t>555-666-8888</t>
+  </si>
+  <si>
+    <t>Shire Bakery</t>
+  </si>
+  <si>
+    <t>Frodo</t>
+  </si>
+  <si>
+    <t>Baggins</t>
+  </si>
+  <si>
+    <t>4 Bag End</t>
+  </si>
+  <si>
+    <t>Frodo@shirebakery.com</t>
+  </si>
+  <si>
+    <t>555-999-0000</t>
+  </si>
+  <si>
+    <t>Rivendell Music</t>
+  </si>
+  <si>
+    <t>Lindir</t>
+  </si>
+  <si>
+    <t>Elf</t>
+  </si>
+  <si>
+    <t>2 Rivendell Way</t>
+  </si>
+  <si>
+    <t>Lindir@rivendellmusic.com</t>
+  </si>
+  <si>
+    <t>Beorn's Honey</t>
+  </si>
+  <si>
+    <t>Beorn</t>
+  </si>
+  <si>
+    <t>Skin-changer</t>
+  </si>
+  <si>
+    <t>300 Honey Lane</t>
+  </si>
+  <si>
+    <t>Carrock</t>
+  </si>
+  <si>
+    <t>Vale of Anduin</t>
+  </si>
+  <si>
+    <t>Beorn@beornshoney.com</t>
+  </si>
+  <si>
+    <t>Dale Carpentry</t>
+  </si>
+  <si>
+    <t>Bard</t>
+  </si>
+  <si>
+    <t>the Bowman</t>
+  </si>
+  <si>
+    <t>200 Lake Street</t>
+  </si>
+  <si>
+    <t>Dale</t>
+  </si>
+  <si>
+    <t>Bard@dalecarpentry.com</t>
+  </si>
+  <si>
+    <t>555-555-6666</t>
+  </si>
+  <si>
+    <t>Lothlorien Looms</t>
+  </si>
+  <si>
+    <t>Galadriel</t>
+  </si>
+  <si>
+    <t>Nenya</t>
+  </si>
+  <si>
+    <t>1000 Lothlorien Way</t>
+  </si>
+  <si>
+    <t>Lothlorien</t>
+  </si>
+  <si>
+    <t>Galadriel@lothlorienlooms.com</t>
+  </si>
+  <si>
+    <t>555-777-8888</t>
+  </si>
+  <si>
+    <t>Bree Inn</t>
+  </si>
+  <si>
+    <t>Barliman</t>
+  </si>
+  <si>
+    <t>Butterbur</t>
+  </si>
+  <si>
+    <t>1 Bree Path</t>
+  </si>
+  <si>
+    <t>Bree</t>
+  </si>
+  <si>
+    <t>Barliman@breeinn.com</t>
+  </si>
+  <si>
+    <t>555-999-1111</t>
   </si>
 </sst>
 </file>
@@ -963,6 +1167,266 @@
         <v>99</v>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>167</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>